<commit_message>
huge changes.. added rate card predictor
</commit_message>
<xml_diff>
--- a/data/UI_sheet.xlsx
+++ b/data/UI_sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sandrarhee/Documents/GitHub/Negotiation_Assistant_UI/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64BA9F2D-1B24-FE4E-996A-9162752954FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D916684-57B2-734A-9F8B-0B333AC5576B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="5" xr2:uid="{26FA3322-B746-8046-862E-CBC756C3B5EA}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" firstSheet="2" activeTab="5" xr2:uid="{26FA3322-B746-8046-862E-CBC756C3B5EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Subcategory_Info" sheetId="12" r:id="rId1"/>
@@ -26,7 +26,7 @@
     <sheet name="Negotiation Levers" sheetId="8" r:id="rId11"/>
     <sheet name="Contract Types" sheetId="9" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1568,7 +1568,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -1676,7 +1676,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -4244,7 +4243,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="A1:C5"/>
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -4927,9 +4926,9 @@
   <sheetPr>
     <tabColor theme="6" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:J29"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
@@ -5071,227 +5070,14 @@
       <c r="H7" s="22"/>
     </row>
     <row r="8" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="49" t="s">
+      <c r="A8" t="s">
         <v>431</v>
       </c>
-      <c r="B8" s="49"/>
-      <c r="C8" s="49"/>
-      <c r="D8" s="49"/>
-      <c r="E8" s="49"/>
-      <c r="F8" s="49"/>
-      <c r="G8" s="49"/>
-      <c r="H8" s="49"/>
-    </row>
-    <row r="9" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="49"/>
-      <c r="B9" s="49"/>
-      <c r="C9" s="49"/>
-      <c r="D9" s="49"/>
-      <c r="E9" s="49"/>
-      <c r="F9" s="49"/>
-      <c r="G9" s="49"/>
-      <c r="H9" s="49"/>
-    </row>
-    <row r="10" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="49"/>
-      <c r="B10" s="49"/>
-      <c r="C10" s="49"/>
-      <c r="D10" s="49"/>
-      <c r="E10" s="49"/>
-      <c r="F10" s="49"/>
-      <c r="G10" s="49"/>
-      <c r="H10" s="49"/>
-    </row>
-    <row r="11" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="49"/>
-      <c r="B11" s="49"/>
-      <c r="C11" s="49"/>
-      <c r="D11" s="49"/>
-      <c r="E11" s="49"/>
-      <c r="F11" s="49"/>
-      <c r="G11" s="49"/>
-      <c r="H11" s="49"/>
-    </row>
-    <row r="12" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="49"/>
-      <c r="B12" s="49"/>
-      <c r="C12" s="49"/>
-      <c r="D12" s="49"/>
-      <c r="E12" s="49"/>
-      <c r="F12" s="49"/>
-      <c r="G12" s="49"/>
-      <c r="H12" s="49"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" s="49"/>
-      <c r="B13" s="49"/>
-      <c r="C13" s="49"/>
-      <c r="D13" s="49"/>
-      <c r="E13" s="49"/>
-      <c r="F13" s="49"/>
-      <c r="G13" s="49"/>
-      <c r="H13" s="49"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" s="49"/>
-      <c r="B14" s="49"/>
-      <c r="C14" s="49"/>
-      <c r="D14" s="49"/>
-      <c r="E14" s="49"/>
-      <c r="F14" s="49"/>
-      <c r="G14" s="49"/>
-      <c r="H14" s="49"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" s="49"/>
-      <c r="B15" s="49"/>
-      <c r="C15" s="49"/>
-      <c r="D15" s="49"/>
-      <c r="E15" s="49"/>
-      <c r="F15" s="49"/>
-      <c r="G15" s="49"/>
-      <c r="H15" s="49"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" s="49"/>
-      <c r="B16" s="49"/>
-      <c r="C16" s="49"/>
-      <c r="D16" s="49"/>
-      <c r="E16" s="49"/>
-      <c r="F16" s="49"/>
-      <c r="G16" s="49"/>
-      <c r="H16" s="49"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" s="49"/>
-      <c r="B17" s="49"/>
-      <c r="C17" s="49"/>
-      <c r="D17" s="49"/>
-      <c r="E17" s="49"/>
-      <c r="F17" s="49"/>
-      <c r="G17" s="49"/>
-      <c r="H17" s="49"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" s="49"/>
-      <c r="B18" s="49"/>
-      <c r="C18" s="49"/>
-      <c r="D18" s="49"/>
-      <c r="E18" s="49"/>
-      <c r="F18" s="49"/>
-      <c r="G18" s="49"/>
-      <c r="H18" s="49"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" s="49"/>
-      <c r="B19" s="49"/>
-      <c r="C19" s="49"/>
-      <c r="D19" s="49"/>
-      <c r="E19" s="49"/>
-      <c r="F19" s="49"/>
-      <c r="G19" s="49"/>
-      <c r="H19" s="49"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" s="49"/>
-      <c r="B20" s="49"/>
-      <c r="C20" s="49"/>
-      <c r="D20" s="49"/>
-      <c r="E20" s="49"/>
-      <c r="F20" s="49"/>
-      <c r="G20" s="49"/>
-      <c r="H20" s="49"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" s="49"/>
-      <c r="B21" s="49"/>
-      <c r="C21" s="49"/>
-      <c r="D21" s="49"/>
-      <c r="E21" s="49"/>
-      <c r="F21" s="49"/>
-      <c r="G21" s="49"/>
-      <c r="H21" s="49"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" s="49"/>
-      <c r="B22" s="49"/>
-      <c r="C22" s="49"/>
-      <c r="D22" s="49"/>
-      <c r="E22" s="49"/>
-      <c r="F22" s="49"/>
-      <c r="G22" s="49"/>
-      <c r="H22" s="49"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" s="49"/>
-      <c r="B23" s="49"/>
-      <c r="C23" s="49"/>
-      <c r="D23" s="49"/>
-      <c r="E23" s="49"/>
-      <c r="F23" s="49"/>
-      <c r="G23" s="49"/>
-      <c r="H23" s="49"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" s="49"/>
-      <c r="B24" s="49"/>
-      <c r="C24" s="49"/>
-      <c r="D24" s="49"/>
-      <c r="E24" s="49"/>
-      <c r="F24" s="49"/>
-      <c r="G24" s="49"/>
-      <c r="H24" s="49"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" s="49"/>
-      <c r="B25" s="49"/>
-      <c r="C25" s="49"/>
-      <c r="D25" s="49"/>
-      <c r="E25" s="49"/>
-      <c r="F25" s="49"/>
-      <c r="G25" s="49"/>
-      <c r="H25" s="49"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" s="49"/>
-      <c r="B26" s="49"/>
-      <c r="C26" s="49"/>
-      <c r="D26" s="49"/>
-      <c r="E26" s="49"/>
-      <c r="F26" s="49"/>
-      <c r="G26" s="49"/>
-      <c r="H26" s="49"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" s="49"/>
-      <c r="B27" s="49"/>
-      <c r="C27" s="49"/>
-      <c r="D27" s="49"/>
-      <c r="E27" s="49"/>
-      <c r="F27" s="49"/>
-      <c r="G27" s="49"/>
-      <c r="H27" s="49"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" s="49"/>
-      <c r="B28" s="49"/>
-      <c r="C28" s="49"/>
-      <c r="D28" s="49"/>
-      <c r="E28" s="49"/>
-      <c r="F28" s="49"/>
-      <c r="G28" s="49"/>
-      <c r="H28" s="49"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29" s="49"/>
-      <c r="B29" s="49"/>
-      <c r="C29" s="49"/>
-      <c r="D29" s="49"/>
-      <c r="E29" s="49"/>
-      <c r="F29" s="49"/>
-      <c r="G29" s="49"/>
-      <c r="H29" s="49"/>
-    </row>
+    </row>
+    <row r="9" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5410,7 +5196,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5532,7 +5318,7 @@
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -5736,9 +5522,7 @@
   </sheetPr>
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>